<commit_message>
add category VIP and fix some bugs
</commit_message>
<xml_diff>
--- a/App/Data_manager/Data/data.xlsx
+++ b/App/Data_manager/Data/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Karaoke_App\Karaoke_app\App\Data_manager\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBD97B2-3175-490A-A51A-AAB8CB61A01D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12B66B9-841D-4C1E-8751-A325DF4BC157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>Tên</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t>Stt</t>
+  </si>
+  <si>
+    <t>thời gian(VIP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">không được phep thay đổi tên của thời gian </t>
   </si>
 </sst>
 </file>
@@ -258,16 +264,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -493,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1008"/>
+  <dimension ref="A1:F1008"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -522,7 +524,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2">
@@ -536,7 +538,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>52</v>
       </c>
       <c r="B3" s="1">
@@ -550,7 +552,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1">
@@ -578,7 +580,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="10" t="s">
         <v>51</v>
       </c>
       <c r="B6" s="2">
@@ -634,7 +636,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="1">
@@ -704,7 +706,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="1">
@@ -731,7 +733,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="14.25" customHeight="1">
+    <row r="17" spans="1:6" ht="14.25" customHeight="1">
       <c r="A17" s="5" t="s">
         <v>22</v>
       </c>
@@ -745,7 +747,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="14.25" customHeight="1">
+    <row r="18" spans="1:6" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -759,11 +761,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A19" s="10" t="s">
+    <row r="19" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A19" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="8">
         <v>150000</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -773,11 +775,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A20" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="8">
         <v>5000</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -787,7 +789,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="14.25" customHeight="1">
+    <row r="21" spans="1:6" ht="14.25" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -801,7 +803,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="14.25" customHeight="1">
+    <row r="22" spans="1:6" ht="14.25" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
@@ -815,8 +817,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A23" s="11" t="s">
+    <row r="23" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A23" s="9" t="s">
         <v>49</v>
       </c>
       <c r="B23" s="1">
@@ -829,8 +831,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A24" s="11" t="s">
+    <row r="24" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A24" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B24" s="1">
@@ -843,7 +845,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="14.25" customHeight="1">
+    <row r="25" spans="1:6" ht="14.25" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -857,8 +859,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A26" s="11" t="s">
+    <row r="26" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A26" s="9" t="s">
         <v>48</v>
       </c>
       <c r="B26" s="1">
@@ -871,7 +873,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="14.25" customHeight="1">
+    <row r="27" spans="1:6" ht="14.25" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>46</v>
       </c>
@@ -884,16 +886,28 @@
       <c r="D27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A28" s="7"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:4" ht="14.25" customHeight="1"/>
+      <c r="F27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="2">
+        <v>250000</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:6" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>

</xml_diff>